<commit_message>
1745 CSV file added
</commit_message>
<xml_diff>
--- a/Models/models.xlsx
+++ b/Models/models.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tugberk\source\repos\Traffic Flow Speed Estimation\Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atlin\PycharmProjects\Traffic-Flow-Estimation\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4835E2-F72D-4CFE-95E5-DDC1A91BE92A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5A6049F-CE4E-48ED-B4E6-8DC52C994064}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" xr2:uid="{0A0C8B08-9AF0-49EC-B3A9-0F2C579D4185}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>MODEL ID</t>
   </si>
@@ -130,6 +130,24 @@
   <si>
     <t>Almost the same with #2. Unneccesary comlexity
 #2 is already ok.</t>
+  </si>
+  <si>
+    <t>2_442</t>
+  </si>
+  <si>
+    <t>1_471</t>
+  </si>
+  <si>
+    <t>2_471</t>
+  </si>
+  <si>
+    <t>3_471</t>
+  </si>
+  <si>
+    <t>4_471</t>
+  </si>
+  <si>
+    <t>5_471</t>
   </si>
 </sst>
 </file>
@@ -184,74 +202,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -268,10 +218,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFF00"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="000000"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -560,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961A103A-7112-41E9-A44C-84DC895BFD54}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -615,8 +565,8 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
+      <c r="A2" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
@@ -653,8 +603,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
+      <c r="A3" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -691,8 +641,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>3</v>
+      <c r="A4" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
@@ -729,8 +679,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>4</v>
+      <c r="A5" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
@@ -767,8 +717,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>54</v>
+      <c r="A6" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>9</v>
@@ -802,6 +752,41 @@
       </c>
       <c r="L6" s="2" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="56.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="1">
+        <v>30</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="1">
+        <v>15.581099999999999</v>
+      </c>
+      <c r="J7" s="1">
+        <v>27.225999999999999</v>
+      </c>
+      <c r="K7" s="1">
+        <v>24.280687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correct mistake on build_model.build_sets and remove corrupted data
</commit_message>
<xml_diff>
--- a/Models/models.xlsx
+++ b/Models/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tugberk\source\repos\Traffic Flow Speed Estimation\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C551269-3762-4091-B654-8FD56A86DE27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FEB120-5EFC-4CD5-B15D-8340E8ECBEDC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" xr2:uid="{0A0C8B08-9AF0-49EC-B3A9-0F2C579D4185}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>MODEL ID</t>
   </si>
@@ -59,92 +59,16 @@
     <t>RUSH ER.</t>
   </si>
   <si>
-    <t>Scaled Speed
-Weekdays oh
-Daypart oh</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
-    <t>Second week
-of May</t>
-  </si>
-  <si>
-    <t>1 WEEK</t>
-  </si>
-  <si>
-    <t>15m Back
-15m Forward</t>
-  </si>
-  <si>
     <t>TEST ERROR</t>
   </si>
   <si>
     <t>TRAIN ERROR</t>
   </si>
   <si>
-    <t>Starting from
-16 of March, 8, up to end of May</t>
-  </si>
-  <si>
-    <t>First 7 days of June</t>
-  </si>
-  <si>
     <t>COMMENT</t>
   </si>
   <si>
-    <t>Base Nodel.</t>
-  </si>
-  <si>
-    <t>Trining set has been increased to 2.5 months
-compared to model #1. It can be seen that this
-has effected the results significantly.</t>
-  </si>
-  <si>
-    <t>2h Back
-2h Forward</t>
-  </si>
-  <si>
-    <t>Time steps has been increased. Though it didn't
-deccrease the loss. Maybe more data is needed
-since there can be more patterns.</t>
-  </si>
-  <si>
-    <t>1h Back
-30m Forward</t>
-  </si>
-  <si>
-    <t>90 minutes time steps is better than 4 hours.
-Almost same with 30 minutes Which one is better? Maybe more complex net will improve this.</t>
-  </si>
-  <si>
-    <t>LSTM(50)+dro(0.5)
-LSTM(50)+dro(0.5)
-LSTM(33)</t>
-  </si>
-  <si>
-    <t>30m Back
-15m Forward</t>
-  </si>
-  <si>
-    <t>Almost the same with #2. Unneccesary comlexity
-#2 is already ok.</t>
-  </si>
-  <si>
     <t>SPEED ID</t>
-  </si>
-  <si>
-    <t>Changing the dataset and using different sensor
-increased the error dramatically. Should try 
-at least one more to understand which one is common</t>
-  </si>
-  <si>
-    <t>it seems like id = 471 was just lucky id. Errors are 
-normally higher that 15%</t>
-  </si>
-  <si>
-    <t>After unsuccefull tries with different sensor points, time step is increased to see if it would help. But there is not any significant improve.</t>
   </si>
 </sst>
 </file>
@@ -577,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961A103A-7112-41E9-A44C-84DC895BFD54}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H1" activeCellId="1" sqref="A1:C4 H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -596,7 +520,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -620,345 +544,93 @@
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>471</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="1">
-        <v>30</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="2">
-        <v>13.85</v>
-      </c>
-      <c r="K2" s="2">
-        <v>21.07</v>
-      </c>
-      <c r="L2" s="1">
-        <v>42.64</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1">
-        <v>471</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="1">
-        <v>30</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="2">
-        <v>14.03</v>
-      </c>
-      <c r="K3" s="2">
-        <v>14.68</v>
-      </c>
-      <c r="L3" s="1">
-        <v>21.07</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>442</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="1">
-        <v>30</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="1">
-        <v>15.581099999999999</v>
-      </c>
-      <c r="K4" s="1">
-        <v>27.225999999999999</v>
-      </c>
-      <c r="L4" s="1">
-        <v>24.280687</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1745</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1">
-        <v>30</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="2">
-        <v>22.95</v>
-      </c>
-      <c r="K5" s="2">
-        <v>27.73</v>
-      </c>
-      <c r="L5" s="1">
-        <v>45.85</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1">
-        <v>471</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="1">
-        <v>30</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="2">
-        <v>13.36</v>
-      </c>
-      <c r="K6" s="2">
-        <v>16.29</v>
-      </c>
-      <c r="L6" s="1">
-        <v>28.38</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1">
-        <v>471</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="1">
-        <v>30</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="2">
-        <v>12.89</v>
-      </c>
-      <c r="K7" s="2">
-        <v>14.29</v>
-      </c>
-      <c r="L7" s="1">
-        <v>24.27</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1745</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="1">
-        <v>30</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="2">
-        <v>21.77</v>
-      </c>
-      <c r="K8" s="2">
-        <v>26.25</v>
-      </c>
-      <c r="L8" s="1">
-        <v>40.729999999999997</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1">
-        <v>471</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="1">
-        <v>50</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="2">
-        <v>12.03</v>
-      </c>
-      <c r="K9" s="2">
-        <v>14.42</v>
-      </c>
-      <c r="L9" s="1">
-        <v>23.52</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="M9" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A2:M9">

</xml_diff>

<commit_message>
Model 3 and 4 added
</commit_message>
<xml_diff>
--- a/Models/models.xlsx
+++ b/Models/models.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tugberk\source\repos\Traffic Flow Speed Estimation\Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atlin\PycharmProjects\Traffic-Flow-Estimation\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4684A0-719D-4C36-AC63-F267275879DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2803C13A-1342-4DC0-BD44-DD514C0BF59E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" xr2:uid="{0A0C8B08-9AF0-49EC-B3A9-0F2C579D4185}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>MODEL ID</t>
   </si>
@@ -104,6 +104,21 @@
   </si>
   <si>
     <t>Increasing the time steps has not changed anytinh.  Model still can't learn after the first epoch. It needs more data.</t>
+  </si>
+  <si>
+    <t>Feb March April May</t>
+  </si>
+  <si>
+    <t>Increasing the training data hasn't done much on improving the accuracy. The increase is so slight that it can be ignored</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Same data set gave a greater loss than 471 for 1745. </t>
+  </si>
+  <si>
+    <t>Feb March April May Oct Nov</t>
+  </si>
+  <si>
+    <t>Increasing training data for 1745 has improved its performance some</t>
   </si>
 </sst>
 </file>
@@ -158,74 +173,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -242,10 +189,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFF00"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="000000"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -536,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961A103A-7112-41E9-A44C-84DC895BFD54}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -674,32 +621,127 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>471</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1">
+        <v>50</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="1">
+        <v>12.95</v>
+      </c>
+      <c r="K4" s="1">
+        <v>16.012</v>
+      </c>
+      <c r="L4" s="1">
+        <v>24</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1745</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1">
+        <v>50</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="2">
+        <v>22.98</v>
+      </c>
+      <c r="K5" s="2">
+        <v>27.8</v>
+      </c>
+      <c r="L5" s="1">
+        <v>22.4</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1745</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1">
+        <v>50</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="2">
+        <v>23.99</v>
+      </c>
+      <c r="K6" s="2">
+        <v>23.67</v>
+      </c>
+      <c r="L6" s="1">
+        <v>27.6</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="2"/>

</xml_diff>

<commit_message>
add Model 6 for ID 471
</commit_message>
<xml_diff>
--- a/Models/models.xlsx
+++ b/Models/models.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atlin\PycharmProjects\Traffic-Flow-Estimation\Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tugberk\source\repos\Traffic Flow Speed Estimation\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB320BD-B9B7-493D-A9E8-3B2C3256168D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA27292A-2AE1-42A9-BA18-4778E53C2F21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" xr2:uid="{0A0C8B08-9AF0-49EC-B3A9-0F2C579D4185}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
   <si>
     <t>MODEL ID</t>
   </si>
@@ -135,6 +135,10 @@
   </si>
   <si>
     <t>Adding a two prev week hasn’t change loss</t>
+  </si>
+  <si>
+    <t>1 week + 
+2 week</t>
   </si>
 </sst>
 </file>
@@ -189,6 +193,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -205,10 +277,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="FFFF00"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="000000"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -499,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961A103A-7112-41E9-A44C-84DC895BFD54}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -819,8 +891,8 @@
       <c r="F8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>16</v>
+      <c r="G8" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>17</v>
@@ -841,15 +913,46 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="M9" s="2"/>
+    <row r="9" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1">
+        <v>471</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1">
+        <v>30</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="2">
+        <v>12.69</v>
+      </c>
+      <c r="K9" s="2">
+        <v>14.6</v>
+      </c>
+      <c r="L9" s="1">
+        <v>23.29</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:M9">

</xml_diff>

<commit_message>
Add versions of Model 1 and 5
</commit_message>
<xml_diff>
--- a/Models/models.xlsx
+++ b/Models/models.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tugberk\source\repos\Traffic Flow Speed Estimation\Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atlin\PycharmProjects\Traffic-Flow-Estimation\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA27292A-2AE1-42A9-BA18-4778E53C2F21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3774FD2E-7F83-4775-A6B6-7E49877DBC10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" xr2:uid="{0A0C8B08-9AF0-49EC-B3A9-0F2C579D4185}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
   <si>
     <t>MODEL ID</t>
   </si>
@@ -139,6 +139,40 @@
   <si>
     <t>1 week + 
 2 week</t>
+  </si>
+  <si>
+    <t>5_v1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scaled speed weeakday o.h hours o.h minute o.h </t>
+  </si>
+  <si>
+    <t>Feb March May April Nov Dec</t>
+  </si>
+  <si>
+    <t>First 7 days of Dec</t>
+  </si>
+  <si>
+    <t>1_v1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200 epoch has not made a seen change on 471 </t>
+  </si>
+  <si>
+    <t>200 epoch has made quite a decrease on train loss but no change on vall los</t>
+  </si>
+  <si>
+    <t>1_V2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feb March May April </t>
+  </si>
+  <si>
+    <t>1_V3</t>
+  </si>
+  <si>
+    <t>30m back
+30m forward</t>
   </si>
 </sst>
 </file>
@@ -193,74 +227,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -277,10 +243,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="FFFF00"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="000000"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -569,18 +535,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961A103A-7112-41E9-A44C-84DC895BFD54}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="9.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" style="1" customWidth="1"/>
-    <col min="5" max="12" width="9.42578125" style="1" customWidth="1"/>
+    <col min="5" max="7" width="9.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="1" customWidth="1"/>
+    <col min="10" max="12" width="9.42578125" style="1" customWidth="1"/>
     <col min="13" max="13" width="31" style="1" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -952,6 +921,164 @@
       </c>
       <c r="M9" s="2" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1745</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1">
+        <v>200</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="1">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="K10" s="1">
+        <v>24.83</v>
+      </c>
+      <c r="L10" s="1">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="1">
+        <v>471</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="1">
+        <v>200</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="K11" s="1">
+        <v>16.3</v>
+      </c>
+      <c r="L11" s="1">
+        <v>25.62</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1">
+        <v>471</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1">
+        <v>200</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="1">
+        <v>12.26</v>
+      </c>
+      <c r="K12" s="1">
+        <v>19.809999999999999</v>
+      </c>
+      <c r="L12" s="1">
+        <v>31.37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1">
+        <v>471</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="1">
+        <v>200</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="1">
+        <v>11.88</v>
+      </c>
+      <c r="K13" s="1">
+        <v>17.850000000000001</v>
+      </c>
+      <c r="L13" s="1">
+        <v>27.85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resolve indentation problem on build_model.py add Model_7 for ID = 1745
</commit_message>
<xml_diff>
--- a/Models/models.xlsx
+++ b/Models/models.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atlin\PycharmProjects\Traffic-Flow-Estimation\Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tugberk\source\repos\Traffic Flow Speed Estimation\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3774FD2E-7F83-4775-A6B6-7E49877DBC10}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8674B277-3FC6-4586-806E-AB5D51D49EED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" xr2:uid="{0A0C8B08-9AF0-49EC-B3A9-0F2C579D4185}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="46">
   <si>
     <t>MODEL ID</t>
   </si>
@@ -173,6 +173,14 @@
   <si>
     <t>30m back
 30m forward</t>
+  </si>
+  <si>
+    <t>1 week+
+2 week+
+3 week</t>
+  </si>
+  <si>
+    <t>Adding 3 week before the estimation hour decreased the success instead of increasing it. Why test loss consistently rises=</t>
   </si>
 </sst>
 </file>
@@ -227,6 +235,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -243,10 +319,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="FFFF00"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="000000"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -535,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961A103A-7112-41E9-A44C-84DC895BFD54}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="G13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1081,6 +1157,47 @@
         <v>27.85</v>
       </c>
     </row>
+    <row r="14" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1745</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1">
+        <v>100</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="2">
+        <v>20.11</v>
+      </c>
+      <c r="K14" s="2">
+        <v>37.409999999999997</v>
+      </c>
+      <c r="L14" s="1">
+        <v>59.076000000000001</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:M9">
     <sortCondition ref="A2:A9"/>

</xml_diff>

<commit_message>
add Model_8 id = 471
</commit_message>
<xml_diff>
--- a/Models/models.xlsx
+++ b/Models/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tugberk\source\repos\Traffic Flow Speed Estimation\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8674B277-3FC6-4586-806E-AB5D51D49EED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433CCDA9-6BC9-4BC0-88A8-4510EC52823B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" xr2:uid="{0A0C8B08-9AF0-49EC-B3A9-0F2C579D4185}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="48">
   <si>
     <t>MODEL ID</t>
   </si>
@@ -181,6 +181,13 @@
   </si>
   <si>
     <t>Adding 3 week before the estimation hour decreased the success instead of increasing it. Why test loss consistently rises=</t>
+  </si>
+  <si>
+    <t>scaled speed of id = 471
+scaled speed of id = 470</t>
+  </si>
+  <si>
+    <t>Adding close sensor sequence didn't change anything. Nothing seems like changing anything.</t>
   </si>
 </sst>
 </file>
@@ -611,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961A103A-7112-41E9-A44C-84DC895BFD54}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="E13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1198,6 +1205,47 @@
         <v>45</v>
       </c>
     </row>
+    <row r="15" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1">
+        <v>471</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1">
+        <v>100</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="2">
+        <v>18.2</v>
+      </c>
+      <c r="K15" s="2">
+        <v>16.18</v>
+      </c>
+      <c r="L15" s="1">
+        <v>26.47</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:M9">
     <sortCondition ref="A2:A9"/>

</xml_diff>